<commit_message>
update data and template
</commit_message>
<xml_diff>
--- a/src/CoronaDataHelper/CoronaDataHelper/res/deathCalculation.xlsx
+++ b/src/CoronaDataHelper/CoronaDataHelper/res/deathCalculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\coronaDataHelper\src\CoronaDataHelper\CoronaDataHelper\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\coronaDataHelper\src\CoronaDataHelper\CoronaDataHelper\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235BDB20-1E90-40F1-81E7-799C17B82DFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362DF926-78F7-4492-9711-19620D686ED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{233D17F4-F1C4-4491-B917-535F87026414}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{233D17F4-F1C4-4491-B917-535F87026414}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -128,11 +128,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#\ ###\ ##0\ ;\-#\ ###\ ##0\ ;&quot; – &quot;"/>
     <numFmt numFmtId="165" formatCode="0.0000_ ;\-0.0000\ "/>
+    <numFmt numFmtId="166" formatCode="#\ ##0_);\-#\ ##0\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +154,30 @@
       <name val="MetaNormalLF-Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="MetaNormalLF-Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial MT"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="MetaNormalLF-Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +187,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF1C9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,10 +234,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -229,9 +264,20 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Link 2" xfId="6" xr:uid="{2CE29C00-D233-4DAC-8DFD-3FA703809DB2}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{2BEFCE1C-9E02-49C6-A6A9-EE801939F0A9}"/>
+    <cellStyle name="Standard 2" xfId="2" xr:uid="{0F8FE32D-D112-4AB7-97A4-FCD89F15A67F}"/>
+    <cellStyle name="Standard 2 2" xfId="3" xr:uid="{ED7FA843-E5AA-48BC-B577-9266FD8FFAFC}"/>
+    <cellStyle name="Standard 3" xfId="5" xr:uid="{6D419069-2AA0-4F47-BCAB-3D51E78D27BF}"/>
+    <cellStyle name="Standard 3 2" xfId="4" xr:uid="{2ACBE21D-53E2-4514-81E0-18B8CDA5A5F9}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -555,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D2C56B-9DFD-4F24-8031-428339693CF3}">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,1317 +676,1285 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="16">
+        <v>103804</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="P2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="7"/>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
         <v>2020</v>
       </c>
-      <c r="C2" s="3">
-        <v>85384</v>
-      </c>
-      <c r="D2" s="3">
-        <v>80013</v>
-      </c>
-      <c r="E2" s="3">
-        <v>87452</v>
-      </c>
-      <c r="F2" s="3">
-        <v>83845</v>
-      </c>
-      <c r="G2" s="3">
-        <v>75775</v>
-      </c>
-      <c r="H2" s="3">
-        <v>72134</v>
-      </c>
-      <c r="I2" s="3">
-        <v>73756</v>
-      </c>
-      <c r="J2" s="3">
-        <v>78629</v>
-      </c>
-      <c r="K2" s="3">
-        <v>73980</v>
-      </c>
-      <c r="L2" s="3">
-        <v>79431</v>
-      </c>
-      <c r="M2" s="3">
-        <v>85483</v>
-      </c>
-      <c r="N2" s="3">
-        <v>106607</v>
-      </c>
-      <c r="P2" s="3">
+      <c r="C3" s="15">
+        <v>85406</v>
+      </c>
+      <c r="D3" s="15">
+        <v>80018</v>
+      </c>
+      <c r="E3" s="15">
+        <v>87457</v>
+      </c>
+      <c r="F3" s="15">
+        <v>83851</v>
+      </c>
+      <c r="G3" s="15">
+        <v>75780</v>
+      </c>
+      <c r="H3" s="15">
+        <v>72142</v>
+      </c>
+      <c r="I3" s="15">
+        <v>73763</v>
+      </c>
+      <c r="J3" s="15">
+        <v>78638</v>
+      </c>
+      <c r="K3" s="15">
+        <v>73993</v>
+      </c>
+      <c r="L3" s="15">
+        <v>79468</v>
+      </c>
+      <c r="M3" s="15">
+        <v>85623</v>
+      </c>
+      <c r="N3" s="15">
+        <v>107862</v>
+      </c>
+      <c r="P3" s="3">
         <v>83200</v>
       </c>
-      <c r="R2" s="5">
-        <f>SUM(E2:N2)</f>
-        <v>817092</v>
-      </c>
-      <c r="S2" s="5">
-        <f>SUM(C2:N2)</f>
-        <v>982489</v>
-      </c>
-      <c r="T2">
-        <f>S2/(P2*1000/100)</f>
-        <v>1.180876201923077</v>
-      </c>
-      <c r="U2">
-        <f>(P2*1000/100)</f>
+      <c r="R3" s="5">
+        <f>SUM(E3:N3)</f>
+        <v>818577</v>
+      </c>
+      <c r="S3" s="5">
+        <f>SUM(C3:N3)</f>
+        <v>984001</v>
+      </c>
+      <c r="T3">
+        <f>S3/(P3*1000/100)</f>
+        <v>1.1826935096153846</v>
+      </c>
+      <c r="U3">
+        <f>(P3*1000/100)</f>
         <v>832000</v>
       </c>
-      <c r="W2" s="5">
-        <f>S2-$S$4</f>
-        <v>27615</v>
-      </c>
-      <c r="X2" s="8">
-        <f>T2-$T$4</f>
-        <v>3.0688895402882777E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="9">
+      <c r="W3" s="5">
+        <f>S3-$S$5</f>
+        <v>29127</v>
+      </c>
+      <c r="X3" s="8">
+        <f>T3-$T$5</f>
+        <v>3.2506203095190367E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="9">
         <v>2019</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="13">
+      <c r="B4" s="9"/>
+      <c r="C4" s="13">
         <v>85105</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D4" s="13">
         <v>81009</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E4" s="13">
         <v>86739</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F4" s="13">
         <v>77410</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G4" s="13">
         <v>75669</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H4" s="13">
         <v>73483</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I4" s="13">
         <v>76926</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J4" s="13">
         <v>73444</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K4" s="13">
         <v>71022</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L4" s="13">
         <v>77006</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M4" s="13">
         <v>78378</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N4" s="13">
         <v>83329</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="13">
+      <c r="O4" s="9"/>
+      <c r="P4" s="13">
         <v>83167</v>
       </c>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="5">
-        <f t="shared" ref="R3:R6" si="0">SUM(E3:N3)</f>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="5">
+        <f t="shared" ref="R4:R7" si="0">SUM(E4:N4)</f>
         <v>773406</v>
       </c>
-      <c r="S3" s="11">
-        <f>SUM(C3:N3)</f>
+      <c r="S4" s="11">
+        <f>SUM(C4:N4)</f>
         <v>939520</v>
       </c>
-      <c r="T3" s="9">
-        <f t="shared" ref="T3:T14" si="1">S3/(P3*1000/100)</f>
+      <c r="T4" s="9">
+        <f t="shared" ref="T4:T15" si="1">S4/(P4*1000/100)</f>
         <v>1.1296788389625694</v>
       </c>
-      <c r="U3" s="9">
-        <f t="shared" ref="U3:U14" si="2">(P3*1000/100)</f>
+      <c r="U4" s="9">
+        <f t="shared" ref="U4:U15" si="2">(P4*1000/100)</f>
         <v>831670</v>
       </c>
-      <c r="V3" s="9"/>
-      <c r="W3" s="11">
-        <f t="shared" ref="W3:W14" si="3">S3-$S$4</f>
+      <c r="V4" s="9"/>
+      <c r="W4" s="11">
+        <f t="shared" ref="W4:W15" si="3">S4-$S$5</f>
         <v>-15354</v>
       </c>
-      <c r="X3" s="12">
-        <f t="shared" ref="X3:X14" si="4">T3-$T$4</f>
+      <c r="X4" s="12">
+        <f t="shared" ref="X4:X15" si="4">T4-$T$5</f>
         <v>-2.050846755762481E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
-      <c r="A4">
+    <row r="5" spans="1:24">
+      <c r="A5">
         <v>2018</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>84973</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="3">
         <v>85799</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E5" s="3">
         <v>107104</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F5" s="3">
         <v>79539</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="3">
         <v>74648</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H5" s="3">
         <v>69328</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I5" s="3">
         <v>75605</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J5" s="3">
         <v>78370</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K5" s="3">
         <v>69708</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L5" s="3">
         <v>74039</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M5" s="3">
         <v>74762</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N5" s="3">
         <v>80999</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P5" s="3">
         <v>83019</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R5" s="5">
         <f t="shared" si="0"/>
         <v>784102</v>
       </c>
-      <c r="S4" s="5">
-        <f>SUM(C4:N4)</f>
+      <c r="S5" s="5">
+        <f>SUM(C5:N5)</f>
         <v>954874</v>
       </c>
-      <c r="T4">
+      <c r="T5">
         <f t="shared" si="1"/>
         <v>1.1501873065201942</v>
       </c>
-      <c r="U4">
+      <c r="U5">
         <f t="shared" si="2"/>
         <v>830190</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W5" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X4" s="8">
+      <c r="X5" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
-      <c r="A5" s="9">
+    <row r="6" spans="1:24">
+      <c r="A6" s="9">
         <v>2017</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="13">
+      <c r="B6" s="9"/>
+      <c r="C6" s="13">
         <v>96033</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D6" s="13">
         <v>90649</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E6" s="13">
         <v>82934</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F6" s="13">
         <v>73204</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G6" s="13">
         <v>75683</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H6" s="13">
         <v>69644</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I6" s="13">
         <v>71411</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J6" s="13">
         <v>71488</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K6" s="13">
         <v>69391</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L6" s="13">
         <v>75229</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M6" s="13">
         <v>74987</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N6" s="13">
         <v>81610</v>
       </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="13">
+      <c r="O6" s="9"/>
+      <c r="P6" s="13">
         <v>82792</v>
       </c>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="5">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="5">
         <f t="shared" si="0"/>
         <v>745581</v>
       </c>
-      <c r="S5" s="11">
-        <f>SUM(C5:N5)</f>
+      <c r="S6" s="11">
+        <f>SUM(C6:N6)</f>
         <v>932263</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T6" s="9">
         <f t="shared" si="1"/>
         <v>1.1260302927819112</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U6" s="9">
         <f t="shared" si="2"/>
         <v>827920</v>
       </c>
-      <c r="V5" s="9"/>
-      <c r="W5" s="11">
+      <c r="V6" s="9"/>
+      <c r="W6" s="11">
         <f t="shared" si="3"/>
         <v>-22611</v>
       </c>
-      <c r="X5" s="12">
+      <c r="X6" s="12">
         <f t="shared" si="4"/>
         <v>-2.415701373828294E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
-      <c r="A6">
+    <row r="7" spans="1:24">
+      <c r="A7">
         <v>2016</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" s="3">
         <v>81742</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="3">
         <v>76619</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E7" s="3">
         <v>83668</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F7" s="3">
         <v>75315</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G7" s="3">
         <v>74525</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H7" s="3">
         <v>69186</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I7" s="3">
         <v>72122</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J7" s="3">
         <v>71295</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K7" s="3">
         <v>69037</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L7" s="3">
         <v>76001</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M7" s="3">
         <v>77050</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N7" s="3">
         <v>84339</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P7" s="3">
         <v>82522</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R7" s="5">
         <f t="shared" si="0"/>
         <v>752538</v>
       </c>
-      <c r="S6" s="5">
-        <f>SUM(C6:N6)</f>
+      <c r="S7" s="5">
+        <f>SUM(C7:N7)</f>
         <v>910899</v>
       </c>
-      <c r="T6">
+      <c r="T7">
         <f t="shared" si="1"/>
         <v>1.1038256464942682</v>
       </c>
-      <c r="U6">
+      <c r="U7">
         <f t="shared" si="2"/>
         <v>825220</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W7" s="5">
         <f t="shared" si="3"/>
         <v>-43975</v>
       </c>
-      <c r="X6" s="8">
+      <c r="X7" s="8">
         <f t="shared" si="4"/>
         <v>-4.636166002592601E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
-      <c r="A7" s="9">
+    <row r="8" spans="1:24">
+      <c r="A8" s="9">
         <v>2015</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9">
         <v>82176</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9">
         <v>925200</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T8" s="9">
         <f t="shared" si="1"/>
         <v>1.125876168224299</v>
       </c>
-      <c r="U7" s="9">
+      <c r="U8" s="9">
         <f t="shared" si="2"/>
         <v>821760</v>
       </c>
-      <c r="V7" s="9"/>
-      <c r="W7" s="11">
+      <c r="V8" s="9"/>
+      <c r="W8" s="11">
         <f t="shared" si="3"/>
         <v>-29674</v>
       </c>
-      <c r="X7" s="12">
+      <c r="X8" s="12">
         <f t="shared" si="4"/>
         <v>-2.4311138295895152E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
-      <c r="A8">
+    <row r="9" spans="1:24">
+      <c r="A9">
         <v>2014</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10">
         <v>81198</v>
       </c>
-      <c r="S8">
+      <c r="S9">
         <v>868356</v>
       </c>
-      <c r="T8">
+      <c r="T9">
         <f t="shared" si="1"/>
         <v>1.069430281534028</v>
       </c>
-      <c r="U8">
+      <c r="U9">
         <f t="shared" si="2"/>
         <v>811980</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W9" s="5">
         <f t="shared" si="3"/>
         <v>-86518</v>
       </c>
-      <c r="X8" s="8">
+      <c r="X9" s="8">
         <f t="shared" si="4"/>
         <v>-8.0757024986166215E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
-      <c r="A9" s="9">
+    <row r="10" spans="1:24">
+      <c r="A10" s="9">
         <v>2013</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9">
         <v>80767</v>
       </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9">
         <v>893825</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T10" s="9">
         <f t="shared" si="1"/>
         <v>1.1066710413906671</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U10" s="9">
         <f t="shared" si="2"/>
         <v>807670</v>
       </c>
-      <c r="V9" s="9"/>
-      <c r="W9" s="11">
+      <c r="V10" s="9"/>
+      <c r="W10" s="11">
         <f t="shared" si="3"/>
         <v>-61049</v>
       </c>
-      <c r="X9" s="12">
+      <c r="X10" s="12">
         <f t="shared" si="4"/>
         <v>-4.351626512952711E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
-      <c r="A10">
+    <row r="11" spans="1:24">
+      <c r="A11">
         <v>2012</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10">
         <v>80524</v>
       </c>
-      <c r="S10">
+      <c r="S11">
         <v>869582</v>
       </c>
-      <c r="T10">
+      <c r="T11">
         <f t="shared" si="1"/>
         <v>1.07990412796185</v>
       </c>
-      <c r="U10">
+      <c r="U11">
         <f t="shared" si="2"/>
         <v>805240</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W11" s="5">
         <f t="shared" si="3"/>
         <v>-85292</v>
       </c>
-      <c r="X10" s="8">
+      <c r="X11" s="8">
         <f t="shared" si="4"/>
         <v>-7.0283178558344206E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="9">
+    <row r="12" spans="1:24">
+      <c r="A12" s="9">
         <v>2011</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9">
         <v>80328</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9">
         <v>852328</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T12" s="9">
         <f t="shared" si="1"/>
         <v>1.0610596554128076</v>
       </c>
-      <c r="U11" s="9">
+      <c r="U12" s="9">
         <f t="shared" si="2"/>
         <v>803280</v>
       </c>
-      <c r="V11" s="9"/>
-      <c r="W11" s="11">
+      <c r="V12" s="9"/>
+      <c r="W12" s="11">
         <f t="shared" si="3"/>
         <v>-102546</v>
       </c>
-      <c r="X11" s="12">
+      <c r="X12" s="12">
         <f t="shared" si="4"/>
         <v>-8.912765110738663E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
-      <c r="A12">
+    <row r="13" spans="1:24">
+      <c r="A13">
         <v>2010</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10">
         <v>81752</v>
       </c>
-      <c r="S12">
+      <c r="S13">
         <v>858768</v>
       </c>
-      <c r="T12">
+      <c r="T13">
         <f t="shared" si="1"/>
         <v>1.0504550347392112</v>
       </c>
-      <c r="U12">
+      <c r="U13">
         <f t="shared" si="2"/>
         <v>817520</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W13" s="5">
         <f t="shared" si="3"/>
         <v>-96106</v>
       </c>
-      <c r="X12" s="8">
+      <c r="X13" s="8">
         <f t="shared" si="4"/>
         <v>-9.9732271780982984E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
-      <c r="A13" s="9">
+    <row r="14" spans="1:24">
+      <c r="A14" s="9">
         <v>2009</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9">
         <v>81802</v>
       </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9">
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9">
         <v>854544</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T14" s="9">
         <f t="shared" si="1"/>
         <v>1.044649275078849</v>
       </c>
-      <c r="U13" s="9">
+      <c r="U14" s="9">
         <f t="shared" si="2"/>
         <v>818020</v>
       </c>
-      <c r="V13" s="9"/>
-      <c r="W13" s="11">
+      <c r="V14" s="9"/>
+      <c r="W14" s="11">
         <f t="shared" si="3"/>
         <v>-100330</v>
       </c>
-      <c r="X13" s="12">
+      <c r="X14" s="12">
         <f t="shared" si="4"/>
         <v>-0.10553803144134521</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
-      <c r="A14">
+    <row r="15" spans="1:24">
+      <c r="A15">
         <v>2008</v>
       </c>
-      <c r="P14">
+      <c r="P15">
         <v>82002</v>
       </c>
-      <c r="S14">
+      <c r="S15">
         <v>844439</v>
       </c>
-      <c r="T14">
+      <c r="T15">
         <f t="shared" si="1"/>
         <v>1.0297785419867809</v>
       </c>
-      <c r="U14">
+      <c r="U15">
         <f t="shared" si="2"/>
         <v>820020</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W15" s="5">
         <f t="shared" si="3"/>
         <v>-110435</v>
       </c>
-      <c r="X14" s="8">
+      <c r="X15" s="8">
         <f t="shared" si="4"/>
         <v>-0.12040876453341331</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
-      <c r="A17" t="s">
+    <row r="18" spans="1:21">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6">
-        <f>SUM(C3:C6)/4</f>
+      <c r="C18" s="6">
+        <f>SUM(C4:C7)/4</f>
         <v>86963.25</v>
       </c>
-      <c r="D17" s="6">
-        <f t="shared" ref="D17:N17" si="5">SUM(D3:D6)/4</f>
+      <c r="D18" s="6">
+        <f t="shared" ref="D18:N18" si="5">SUM(D4:D7)/4</f>
         <v>83519</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E18" s="6">
         <f t="shared" si="5"/>
         <v>90111.25</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F18" s="6">
         <f t="shared" si="5"/>
         <v>76367</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G18" s="6">
         <f t="shared" si="5"/>
         <v>75131.25</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H18" s="6">
         <f t="shared" si="5"/>
         <v>70410.25</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6">
         <f t="shared" si="5"/>
         <v>74016</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J18" s="6">
         <f t="shared" si="5"/>
         <v>73649.25</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K18" s="6">
         <f t="shared" si="5"/>
         <v>69789.5</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L18" s="6">
         <f t="shared" si="5"/>
         <v>75568.75</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M18" s="6">
         <f t="shared" si="5"/>
         <v>76294.25</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N18" s="6">
         <f t="shared" si="5"/>
         <v>82569.25</v>
       </c>
-      <c r="T17">
-        <f>SUM(S3:S7)/5</f>
+      <c r="T18">
+        <f>SUM(S4:S8)/5</f>
         <v>932551.2</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
-      <c r="A18" t="s">
+    <row r="19" spans="1:21">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5">
-        <f>MEDIAN(C3:C6)</f>
+      <c r="C19" s="5">
+        <f>MEDIAN(C4:C7)</f>
         <v>85039</v>
       </c>
-      <c r="D18" s="5">
-        <f t="shared" ref="D18:N18" si="6">MEDIAN(D3:D6)</f>
+      <c r="D19" s="5">
+        <f t="shared" ref="D19:N19" si="6">MEDIAN(D4:D7)</f>
         <v>83404</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E19" s="5">
         <f t="shared" si="6"/>
         <v>85203.5</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F19" s="5">
         <f t="shared" si="6"/>
         <v>76362.5</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G19" s="5">
         <f t="shared" si="6"/>
         <v>75158.5</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H19" s="5">
         <f t="shared" si="6"/>
         <v>69486</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I19" s="5">
         <f t="shared" si="6"/>
         <v>73863.5</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J19" s="5">
         <f t="shared" si="6"/>
         <v>72466</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K19" s="5">
         <f t="shared" si="6"/>
         <v>69549.5</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L19" s="5">
         <f t="shared" si="6"/>
         <v>75615</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M19" s="5">
         <f t="shared" si="6"/>
         <v>76018.5</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N19" s="5">
         <f t="shared" si="6"/>
         <v>82469.5</v>
       </c>
-      <c r="U18" s="5">
-        <f>S2-T17</f>
-        <v>49937.800000000047</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" t="s">
+      <c r="U19" s="5">
+        <f>S3-T18</f>
+        <v>51449.800000000047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="6">
-        <f>SUM(C4:C6)/3</f>
+      <c r="C21" s="6">
+        <f>SUM(C5:C7)/3</f>
         <v>87582.666666666672</v>
       </c>
-      <c r="D20" s="6">
-        <f t="shared" ref="D20:N20" si="7">SUM(D4:D6)/3</f>
+      <c r="D21" s="6">
+        <f t="shared" ref="D21:N21" si="7">SUM(D5:D7)/3</f>
         <v>84355.666666666672</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E21" s="6">
         <f t="shared" si="7"/>
         <v>91235.333333333328</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F21" s="6">
         <f t="shared" si="7"/>
         <v>76019.333333333328</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G21" s="6">
         <f t="shared" si="7"/>
         <v>74952</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H21" s="6">
         <f t="shared" si="7"/>
         <v>69386</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I21" s="6">
         <f t="shared" si="7"/>
         <v>73046</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J21" s="6">
         <f t="shared" si="7"/>
         <v>73717.666666666672</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K21" s="6">
         <f t="shared" si="7"/>
         <v>69378.666666666672</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L21" s="6">
         <f t="shared" si="7"/>
         <v>75089.666666666672</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M21" s="6">
         <f t="shared" si="7"/>
         <v>75599.666666666672</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N21" s="6">
         <f t="shared" si="7"/>
         <v>82316</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
-      <c r="A21" t="s">
+    <row r="22" spans="1:21">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5">
-        <f>MEDIAN(C4:C6)</f>
+      <c r="C22" s="5">
+        <f>MEDIAN(C5:C7)</f>
         <v>84973</v>
       </c>
-      <c r="D21" s="5">
-        <f t="shared" ref="D21:N21" si="8">MEDIAN(D4:D6)</f>
+      <c r="D22" s="5">
+        <f t="shared" ref="D22:N22" si="8">MEDIAN(D5:D7)</f>
         <v>85799</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E22" s="5">
         <f t="shared" si="8"/>
         <v>83668</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F22" s="5">
         <f t="shared" si="8"/>
         <v>75315</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G22" s="5">
         <f t="shared" si="8"/>
         <v>74648</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H22" s="5">
         <f t="shared" si="8"/>
         <v>69328</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I22" s="5">
         <f t="shared" si="8"/>
         <v>72122</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J22" s="5">
         <f t="shared" si="8"/>
         <v>71488</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K22" s="5">
         <f t="shared" si="8"/>
         <v>69391</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L22" s="5">
         <f t="shared" si="8"/>
         <v>75229</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M22" s="5">
         <f t="shared" si="8"/>
         <v>74987</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N22" s="5">
         <f t="shared" si="8"/>
         <v>81610</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
-      <c r="A24" t="s">
+    <row r="25" spans="1:21">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="6">
-        <f>SUM(C5:C6)/2</f>
+      <c r="C25" s="6">
+        <f>SUM(C6:C7)/2</f>
         <v>88887.5</v>
       </c>
-      <c r="D24" s="6">
-        <f t="shared" ref="D24:N24" si="9">SUM(D5:D6)/2</f>
+      <c r="D25" s="6">
+        <f t="shared" ref="D25:N25" si="9">SUM(D6:D7)/2</f>
         <v>83634</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E25" s="6">
         <f t="shared" si="9"/>
         <v>83301</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F25" s="6">
         <f t="shared" si="9"/>
         <v>74259.5</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G25" s="6">
         <f t="shared" si="9"/>
         <v>75104</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H25" s="6">
         <f t="shared" si="9"/>
         <v>69415</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I25" s="6">
         <f t="shared" si="9"/>
         <v>71766.5</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J25" s="6">
         <f t="shared" si="9"/>
         <v>71391.5</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K25" s="6">
         <f t="shared" si="9"/>
         <v>69214</v>
       </c>
-      <c r="L24" s="6">
+      <c r="L25" s="6">
         <f t="shared" si="9"/>
         <v>75615</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M25" s="6">
         <f t="shared" si="9"/>
         <v>76018.5</v>
       </c>
-      <c r="N24" s="6">
+      <c r="N25" s="6">
         <f t="shared" si="9"/>
         <v>82974.5</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
-      <c r="A25" t="s">
+    <row r="26" spans="1:21">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="5">
-        <f>MEDIAN(C5:C6)</f>
+      <c r="C26" s="5">
+        <f>MEDIAN(C6:C7)</f>
         <v>88887.5</v>
       </c>
-      <c r="D25" s="5">
-        <f t="shared" ref="D25:N25" si="10">MEDIAN(D5:D6)</f>
+      <c r="D26" s="5">
+        <f t="shared" ref="D26:N26" si="10">MEDIAN(D6:D7)</f>
         <v>83634</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E26" s="5">
         <f t="shared" si="10"/>
         <v>83301</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F26" s="5">
         <f t="shared" si="10"/>
         <v>74259.5</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G26" s="5">
         <f t="shared" si="10"/>
         <v>75104</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H26" s="5">
         <f t="shared" si="10"/>
         <v>69415</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I26" s="5">
         <f t="shared" si="10"/>
         <v>71766.5</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J26" s="5">
         <f t="shared" si="10"/>
         <v>71391.5</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K26" s="5">
         <f t="shared" si="10"/>
         <v>69214</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L26" s="5">
         <f t="shared" si="10"/>
         <v>75615</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M26" s="5">
         <f t="shared" si="10"/>
         <v>76018.5</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N26" s="5">
         <f t="shared" si="10"/>
         <v>82974.5</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
-      <c r="A29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29">
-        <f t="shared" ref="C29:N29" si="11">C2/(C17/100)-100</f>
-        <v>-1.8159969872331203</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="11"/>
-        <v>-4.1978471964463182</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="11"/>
-        <v>-2.9510743664081787</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="11"/>
-        <v>9.792187725064494</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="11"/>
-        <v>0.85683387405373423</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="11"/>
-        <v>2.4481520801303844</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="11"/>
-        <v>-0.35127539991353274</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="11"/>
-        <v>6.7614402047542939</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="11"/>
-        <v>6.0044849153526059</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="11"/>
-        <v>5.1109089405342871</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="11"/>
-        <v>12.043830301759314</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="11"/>
-        <v>29.112230037211191</v>
-      </c>
-      <c r="Q29">
-        <f>SUM(C29:N29)/11</f>
-        <v>5.7103521935326507</v>
-      </c>
-    </row>
     <row r="30" spans="1:21">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:N30" si="12">C2/(C18/100)-100</f>
-        <v>0.40569620997425204</v>
+        <f t="shared" ref="C30:N30" si="11">C3/(C18/100)-100</f>
+        <v>-1.7906989446691597</v>
       </c>
       <c r="D30">
-        <f t="shared" si="12"/>
-        <v>-4.0657522420986965</v>
+        <f t="shared" si="11"/>
+        <v>-4.1918605347286331</v>
       </c>
       <c r="E30">
-        <f t="shared" si="12"/>
-        <v>2.6389760983997235</v>
+        <f t="shared" si="11"/>
+        <v>-2.9455256696583376</v>
       </c>
       <c r="F30">
-        <f t="shared" si="12"/>
-        <v>9.7986577181208077</v>
+        <f t="shared" si="11"/>
+        <v>9.8000445218484487</v>
       </c>
       <c r="G30">
-        <f t="shared" si="12"/>
-        <v>0.82026650345602548</v>
+        <f t="shared" si="11"/>
+        <v>0.86348889443473809</v>
       </c>
       <c r="H30">
-        <f t="shared" si="12"/>
-        <v>3.8108395935871897</v>
+        <f t="shared" si="11"/>
+        <v>2.4595140622281662</v>
       </c>
       <c r="I30">
-        <f t="shared" si="12"/>
-        <v>-0.14553873022533992</v>
+        <f t="shared" si="11"/>
+        <v>-0.34181798530046592</v>
       </c>
       <c r="J30">
-        <f t="shared" si="12"/>
-        <v>8.504678055915889</v>
+        <f t="shared" si="11"/>
+        <v>6.7736602884618691</v>
       </c>
       <c r="K30">
-        <f t="shared" si="12"/>
-        <v>6.3702830358234053</v>
+        <f t="shared" si="11"/>
+        <v>6.0231123593090672</v>
       </c>
       <c r="L30">
-        <f t="shared" si="12"/>
-        <v>5.046617734576472</v>
+        <f t="shared" si="11"/>
+        <v>5.1598709784136929</v>
       </c>
       <c r="M30">
-        <f t="shared" si="12"/>
-        <v>12.450258818577069</v>
+        <f t="shared" si="11"/>
+        <v>12.227330368933437</v>
       </c>
       <c r="N30">
-        <f t="shared" si="12"/>
-        <v>29.268396194956921</v>
+        <f t="shared" si="11"/>
+        <v>30.632166333108273</v>
       </c>
       <c r="Q30">
         <f>SUM(C30:N30)/11</f>
-        <v>6.8093980900967015</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33">
-        <f>C3/(C20/100)-100</f>
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="D33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="E33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="F33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="G33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="H33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="I33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="J33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="K33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="L33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="M33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="N33">
-        <v>-2.8289463668610324</v>
-      </c>
-      <c r="Q33">
-        <f>SUM(C33:N33)/11</f>
-        <v>-3.0861233093029443</v>
+        <v>5.8790258793073722</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:N31" si="12">C3/(C19/100)-100</f>
+        <v>0.43156669292912397</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="12"/>
+        <v>-4.0597573257877286</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="12"/>
+        <v>2.6448444019318487</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="12"/>
+        <v>9.8065149779014575</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="12"/>
+        <v>0.82691911094552495</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="12"/>
+        <v>3.822352704141835</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="12"/>
+        <v>-0.1360617896525298</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="12"/>
+        <v>8.5170976733916604</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="12"/>
+        <v>6.3889747589846024</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="12"/>
+        <v>5.0955498247702167</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="12"/>
+        <v>12.634424515085158</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="12"/>
+        <v>30.790170911670373</v>
+      </c>
+      <c r="Q31">
+        <f>SUM(C31:N31)/11</f>
+        <v>6.9784178596646855</v>
       </c>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <f>C3/(C21/100)-100</f>
-        <v>0.15534346204087512</v>
+        <f>C4/(C21/100)-100</f>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="D34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="E34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="F34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="G34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="H34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="I34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="J34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="K34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="L34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="M34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="N34">
-        <v>0.15534346204087512</v>
+        <v>-2.8289463668610324</v>
       </c>
       <c r="Q34">
         <f>SUM(C34:N34)/11</f>
+        <v>-3.0861233093029443</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <f>C4/(C22/100)-100</f>
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="D35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="E35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="F35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="G35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="H35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="I35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="J35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="K35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="L35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="M35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="N35">
+        <v>0.15534346204087512</v>
+      </c>
+      <c r="Q35">
+        <f>SUM(C35:N35)/11</f>
         <v>0.16946559495368196</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
-      <c r="A37" t="s">
+    <row r="38" spans="1:17">
+      <c r="A38" t="s">
         <v>21</v>
       </c>
-      <c r="C37">
-        <f>C4/(C24/100)-100</f>
+      <c r="C38">
+        <f>C5/(C25/100)-100</f>
         <v>-4.4038813106454739</v>
       </c>
-      <c r="D37">
-        <f t="shared" ref="D37:N37" si="13">D4/(D24/100)-100</f>
+      <c r="D38">
+        <f t="shared" ref="D38:N38" si="13">D5/(D25/100)-100</f>
         <v>2.5886601143075723</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <f t="shared" si="13"/>
         <v>28.574686978547675</v>
       </c>
-      <c r="F37">
+      <c r="F38">
         <f t="shared" si="13"/>
         <v>7.109528073849134</v>
       </c>
-      <c r="G37">
+      <c r="G38">
         <f t="shared" si="13"/>
         <v>-0.60715807413718892</v>
       </c>
-      <c r="H37">
+      <c r="H38">
         <f t="shared" si="13"/>
         <v>-0.1253331412518861</v>
       </c>
-      <c r="I37">
+      <c r="I38">
         <f t="shared" si="13"/>
         <v>5.3485957933018966</v>
       </c>
-      <c r="J37">
+      <c r="J38">
         <f t="shared" si="13"/>
         <v>9.7749732110965653</v>
       </c>
-      <c r="K37">
+      <c r="K38">
         <f t="shared" si="13"/>
         <v>0.71372843644348904</v>
       </c>
-      <c r="L37">
+      <c r="L38">
         <f t="shared" si="13"/>
         <v>-2.0842425444686938</v>
       </c>
-      <c r="M37">
+      <c r="M38">
         <f t="shared" si="13"/>
         <v>-1.6528871261600671</v>
       </c>
-      <c r="N37">
+      <c r="N38">
         <f t="shared" si="13"/>
-        <v>-2.3808519484902035</v>
-      </c>
-      <c r="Q37">
-        <f>SUM(C37:N37)/11</f>
-        <v>3.8959834965811653</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38">
-        <f>C4/(C25/100)-100</f>
-        <v>-4.4038813106454739</v>
-      </c>
-      <c r="D38">
-        <f t="shared" ref="D38:N38" si="14">D4/(D25/100)-100</f>
-        <v>2.5886601143075723</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="14"/>
-        <v>28.574686978547675</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="14"/>
-        <v>7.109528073849134</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="14"/>
-        <v>-0.60715807413718892</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="14"/>
-        <v>-0.1253331412518861</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="14"/>
-        <v>5.3485957933018966</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="14"/>
-        <v>9.7749732110965653</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="14"/>
-        <v>0.71372843644348904</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="14"/>
-        <v>-2.0842425444686938</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="14"/>
-        <v>-1.6528871261600671</v>
-      </c>
-      <c r="N38">
-        <f t="shared" si="14"/>
         <v>-2.3808519484902035</v>
       </c>
       <c r="Q38">
@@ -1948,10 +1962,67 @@
         <v>3.8959834965811653</v>
       </c>
     </row>
+    <row r="39" spans="1:17">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <f>C5/(C26/100)-100</f>
+        <v>-4.4038813106454739</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:N39" si="14">D5/(D26/100)-100</f>
+        <v>2.5886601143075723</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="14"/>
+        <v>28.574686978547675</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="14"/>
+        <v>7.109528073849134</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="14"/>
+        <v>-0.60715807413718892</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="14"/>
+        <v>-0.1253331412518861</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="14"/>
+        <v>5.3485957933018966</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="14"/>
+        <v>9.7749732110965653</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="14"/>
+        <v>0.71372843644348904</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="14"/>
+        <v>-2.0842425444686938</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="14"/>
+        <v>-1.6528871261600671</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="14"/>
+        <v>-2.3808519484902035</v>
+      </c>
+      <c r="Q39">
+        <f>SUM(C39:N39)/11</f>
+        <v>3.8959834965811653</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:N14 P2:P14 W2:X14 R2:U14">
+  <conditionalFormatting sqref="C3:N15 P3:P15 W3:X15 R3:U15">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>C2=MAX(C$2:C$6)</formula>
+      <formula>C3=MAX(C$3:C$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>